<commit_message>
correction nom colonne fichier musics
</commit_message>
<xml_diff>
--- a/data/raw/MusicMind - musics used for training.xlsx
+++ b/data/raw/MusicMind - musics used for training.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redh0\PycharmProjects\MusicMind\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2462B136-51C4-4196-B4B0-7336D4D951E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="voici la fin" sheetId="1" r:id="rId4"/>
+    <sheet name="voici la fin" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
-  <si>
-    <t>Genre</t>
-  </si>
-  <si>
-    <t>Musique</t>
-  </si>
-  <si>
-    <t>cla</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Allegro Con Brio</t>
   </si>
@@ -52,9 +52,6 @@
     <t>William Tell Overture (Finale)</t>
   </si>
   <si>
-    <t>met</t>
-  </si>
-  <si>
     <t>Ace of Spades</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>Welcome To Hell</t>
   </si>
   <si>
-    <t>pop</t>
-  </si>
-  <si>
     <t>Another Night</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>Treat You Better</t>
   </si>
   <si>
-    <t>rap</t>
-  </si>
-  <si>
     <t>California Love</t>
   </si>
   <si>
@@ -151,9 +142,6 @@
     <t>Still D.R.E.</t>
   </si>
   <si>
-    <t>roc</t>
-  </si>
-  <si>
     <t>Bohemian Rhapsody</t>
   </si>
   <si>
@@ -182,26 +170,31 @@
   </si>
   <si>
     <t>Whole Lotta Love</t>
+  </si>
+  <si>
+    <t>Nom du fichier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -212,39 +205,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -434,428 +432,278 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="2" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="2" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="2" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="2" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="2" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="2" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="2" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="2" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>